<commit_message>
update GFS data and added colors
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="GFS-HDD" sheetId="1" r:id="rId1"/>
-    <sheet name="ECMWF-HDD" sheetId="2" r:id="rId2"/>
+    <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
+    <sheet name="ECMWF-HDD" sheetId="1" r:id="rId2"/>
     <sheet name="ECMWF-Ensemble-HDD" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>2018-01-02 12z</t>
+  </si>
+  <si>
+    <t>2018-01-03 00z</t>
   </si>
 </sst>
 </file>
@@ -106,8 +109,255 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -403,10 +653,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>43117</v>
+      </c>
+      <c r="B2" s="5">
+        <v>-6.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>43116</v>
+      </c>
+      <c r="B3" s="5">
+        <v>-3.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>43115</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-0.43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>43114</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43113</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>43112</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>43111</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-1.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>43110</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>43109</v>
+      </c>
+      <c r="B10" s="5">
+        <v>-3.86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>43108</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-5.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43107</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>43106</v>
+      </c>
+      <c r="B13" s="5">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43105</v>
+      </c>
+      <c r="B14" s="5">
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>43104</v>
+      </c>
+      <c r="B15" s="5">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43103</v>
+      </c>
+      <c r="B16" s="5">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <f>SUM(B2:B16)</f>
+        <v>35.020000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B16">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,146 +910,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>43116</v>
-      </c>
-      <c r="B2" s="5">
-        <v>-0.21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>43115</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>43114</v>
-      </c>
-      <c r="B4" s="5">
-        <v>4.62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>43113</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>43112</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>43111</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>43110</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>43109</v>
-      </c>
-      <c r="B9" s="5">
-        <v>-1.66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>43108</v>
-      </c>
-      <c r="B10" s="5">
-        <v>-3.16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>43107</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>43106</v>
-      </c>
-      <c r="B12" s="5">
-        <v>12.42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>43105</v>
-      </c>
-      <c r="B13" s="5">
-        <v>13.55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>43104</v>
-      </c>
-      <c r="B14" s="5">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>43103</v>
-      </c>
-      <c r="B15" s="5">
-        <v>10.72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="5">
-        <f>SUM(B2:B15)</f>
-        <v>59.83</v>
-      </c>
-    </row>
-  </sheetData>
+  <conditionalFormatting sqref="B2:B10">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -649,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,6 +1061,14 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B15">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update GFS on 201801051231
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>2018-01-04 00z</t>
+  </si>
+  <si>
+    <t>2018-01-05 00z</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -701,270 +738,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43119</v>
       </c>
       <c r="B2" s="2">
+        <v>-10.98</v>
+      </c>
+      <c r="C2" s="2">
         <v>-10.28</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43118</v>
       </c>
       <c r="B3" s="2">
+        <v>-10.48</v>
+      </c>
+      <c r="C3" s="2">
         <v>-6.81</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43117</v>
       </c>
       <c r="B4" s="2">
+        <v>-8.9</v>
+      </c>
+      <c r="C4" s="2">
         <v>-0.99</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43116</v>
       </c>
       <c r="B5" s="2">
+        <v>-4.1100000000000003</v>
+      </c>
+      <c r="C5" s="2">
         <v>3.95</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>-6.26</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="6" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43115</v>
       </c>
       <c r="B6" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="C6" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43114</v>
       </c>
       <c r="B7" s="2">
+        <v>-1.01</v>
+      </c>
+      <c r="C7" s="2">
         <v>2.29</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>-0.09</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43113</v>
       </c>
       <c r="B8" s="2">
+        <v>-0.66</v>
+      </c>
+      <c r="C8" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>-1.43</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43112</v>
       </c>
       <c r="B9" s="2">
+        <v>2.38</v>
+      </c>
+      <c r="C9" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>-3.52</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43111</v>
       </c>
       <c r="B10" s="2">
+        <v>-4.13</v>
+      </c>
+      <c r="C10" s="2">
         <v>-4.57</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>0.31</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>-1.06</v>
       </c>
     </row>
-    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43110</v>
       </c>
       <c r="B11" s="2">
+        <v>-3.96</v>
+      </c>
+      <c r="C11" s="2">
         <v>-2.85</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>2.44</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="12" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43109</v>
       </c>
       <c r="B12" s="2">
+        <v>-2.52</v>
+      </c>
+      <c r="C12" s="2">
         <v>-2.36</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>-3.49</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>-3.86</v>
       </c>
     </row>
-    <row r="13" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43108</v>
       </c>
       <c r="B13" s="2">
+        <v>-3.15</v>
+      </c>
+      <c r="C13" s="2">
         <v>-3.31</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>-2.99</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>-5.51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43107</v>
       </c>
       <c r="B14" s="2">
+        <v>2.94</v>
+      </c>
+      <c r="C14" s="2">
         <v>3.32</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>3.79</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43106</v>
       </c>
       <c r="B15" s="2">
+        <v>9.02</v>
+      </c>
+      <c r="C15" s="2">
         <v>9.2799999999999994</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>9.9600000000000009</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>9.36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43105</v>
       </c>
       <c r="B16" s="2">
+        <v>9.92</v>
+      </c>
+      <c r="C16" s="2">
         <v>10.26</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>10.46</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>10.94</v>
       </c>
     </row>
-    <row r="17" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43104</v>
       </c>
       <c r="B17" s="2">
         <f>SUM(B2:B16)</f>
+        <v>-27.14</v>
+      </c>
+      <c r="C17" s="2">
+        <f>SUM(C2:C16)</f>
         <v>2.7300000000000004</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>10.3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43103</v>
       </c>
-      <c r="C18" s="2">
-        <f>SUM(C3:C17)</f>
+      <c r="D18" s="2">
+        <f>SUM(D3:D17)</f>
         <v>-2.9999999999997584E-2</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="19" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="2">
-        <f>SUM(D4:D18)</f>
+    <row r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="2">
+        <f>SUM(E4:E18)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D18">
+  <conditionalFormatting sqref="E4:E18">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D17">
     <cfRule type="cellIs" dxfId="27" priority="5" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -972,7 +1070,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C17">
+  <conditionalFormatting sqref="C2:C16">
     <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -998,16 +1096,16 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -1019,29 +1117,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43113</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2">
+        <v>1.19</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43112</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>-1.76</v>
+      </c>
       <c r="C3" s="2">
         <v>-3.11</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43111</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>-5.31</v>
+      </c>
       <c r="C4" s="2">
         <v>2.5499999999999998</v>
       </c>
@@ -1049,11 +1153,13 @@
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43110</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>-1.89</v>
+      </c>
       <c r="C5" s="2">
         <v>4.54</v>
       </c>
@@ -1061,11 +1167,13 @@
         <v>-1.19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43109</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>-1.65</v>
+      </c>
       <c r="C6" s="2">
         <v>0.2</v>
       </c>
@@ -1073,11 +1181,13 @@
         <v>-3.22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43108</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>-1.07</v>
+      </c>
       <c r="C7" s="2">
         <v>0.27</v>
       </c>
@@ -1085,11 +1195,13 @@
         <v>-4.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43107</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>6.26</v>
+      </c>
       <c r="C8" s="2">
         <v>5.21</v>
       </c>
@@ -1097,11 +1209,13 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43106</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>12.27</v>
+      </c>
       <c r="C9" s="2">
         <v>12.63</v>
       </c>
@@ -1109,7 +1223,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43105</v>
       </c>
@@ -1123,13 +1237,13 @@
         <v>13.07</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43104</v>
       </c>
       <c r="B11" s="2">
         <f>SUM(B2:B10)</f>
-        <v>12.23</v>
+        <v>20.27</v>
       </c>
       <c r="C11" s="2">
         <v>11.69</v>
@@ -1138,7 +1252,7 @@
         <v>11.52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43103</v>
       </c>
@@ -1151,7 +1265,7 @@
         <v>10.27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1192,342 +1306,416 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
+        <v>43118</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-7.22</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>43117</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
+        <v>-4.34</v>
+      </c>
+      <c r="C3" s="2">
         <v>-5.25</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="D3" s="2"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>43116</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
+        <v>-0.59</v>
+      </c>
+      <c r="C4" s="2">
         <v>-2.1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D4" s="2">
         <v>-3.32</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E4" s="2">
         <v>-0.98</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F4" s="2">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>43115</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
+        <v>2.73</v>
+      </c>
+      <c r="C5" s="2">
         <v>1.07</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="2">
         <v>0.05</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E5" s="2">
         <v>1.6</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F5" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>43114</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>4.32</v>
+      </c>
+      <c r="C6" s="2">
         <v>3.59</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>2.62</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>3.37</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F6" s="2">
         <v>4.62</v>
       </c>
     </row>
-    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>43113</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="C7" s="2">
         <v>3.63</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>2.06</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>2.59</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>43112</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>-0.08</v>
+      </c>
+      <c r="C8" s="2">
         <v>0.46</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>1.44</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>1.58</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>43111</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>-5.05</v>
+      </c>
+      <c r="C9" s="2">
         <v>-3.31</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>2.34</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>0.63</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>43110</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>-3.68</v>
+      </c>
+      <c r="C10" s="2">
         <v>-2.74</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>1.63</v>
       </c>
     </row>
-    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>43109</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>-2.34</v>
+      </c>
+      <c r="C11" s="2">
         <v>-1.72</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>-0.82</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>-0.25</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>-1.66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>43108</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="C12" s="2">
         <v>-0.92</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>-0.84</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>-1.61</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>-3.16</v>
       </c>
     </row>
-    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>43107</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>6.29</v>
+      </c>
+      <c r="C13" s="2">
         <v>6.25</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>5.26</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>3.76</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>2.85</v>
       </c>
     </row>
-    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>43106</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
+        <v>12.56</v>
+      </c>
+      <c r="C14" s="2">
         <v>12.6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="2">
         <v>13.02</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>12.61</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>12.42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>43105</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>12.51</v>
+      </c>
+      <c r="C15" s="2">
         <v>12.64</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>13.24</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>13.38</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>13.55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>43104</v>
-      </c>
-      <c r="B15" s="2">
-        <v>11.71</v>
-      </c>
-      <c r="C15" s="2">
-        <v>11.91</v>
-      </c>
-      <c r="D15" s="2">
-        <v>11.84</v>
-      </c>
-      <c r="E15" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>43103</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
+        <v>16.470000000000002</v>
+      </c>
+      <c r="C16" s="2">
+        <v>11.71</v>
+      </c>
+      <c r="D16" s="2">
+        <v>11.91</v>
+      </c>
+      <c r="E16" s="2">
+        <v>11.84</v>
+      </c>
+      <c r="F16" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>43103</v>
+      </c>
+      <c r="C17" s="2">
+        <f>SUM(C3:C16)</f>
         <v>35.909999999999997</v>
       </c>
-      <c r="C16" s="2">
-        <f>SUM(C2:C15)</f>
-        <v>49.22</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10.97</v>
-      </c>
-      <c r="E16" s="2">
-        <v>10.72</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="2">
         <f>SUM(D3:D16)</f>
+        <v>49.22</v>
+      </c>
+      <c r="E17" s="2">
+        <v>10.97</v>
+      </c>
+      <c r="F17" s="2">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="2">
+        <f>SUM(E4:E17)</f>
         <v>60.58</v>
       </c>
-      <c r="E17" s="2">
-        <f>SUM(E3:E16)</f>
+      <c r="F18" s="2">
+        <f>SUM(F4:F17)</f>
         <v>59.83</v>
       </c>
     </row>
-    <row r="18" spans="4:5" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="D3:E16">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="E4:F17">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E17">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D16">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="C3:C16">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="C3:C16">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="B3:B15">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B15">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update gfs on 201801080059
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>2018-01-05 00z</t>
+  </si>
+  <si>
+    <t>2018-01-08 00z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01-07 12z </t>
   </si>
 </sst>
 </file>
@@ -129,7 +135,194 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -738,351 +931,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>43119</v>
+        <v>43122</v>
       </c>
       <c r="B2" s="2">
-        <v>-10.98</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-10.28</v>
-      </c>
+        <v>1.91</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
+        <v>43121</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-0.15</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>43120</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.85</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>43119</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-10.98</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-10.28</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>43118</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B6" s="2">
+        <v>6.76</v>
+      </c>
+      <c r="C6" s="2">
         <v>-10.48</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D6" s="2">
         <v>-6.81</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E6" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>43117</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B7" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="C7" s="2">
         <v>-8.9</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D7" s="2">
         <v>-0.99</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E7" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F7" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>43116</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2">
+        <v>4.46</v>
+      </c>
+      <c r="C8" s="2">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D8" s="2">
         <v>3.95</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E8" s="2">
         <v>-6.26</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F8" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>43115</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B9" s="2">
+        <v>9.85</v>
+      </c>
+      <c r="C9" s="2">
         <v>-1.5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D9" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E9" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F9" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>43114</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B10" s="2">
+        <v>9.44</v>
+      </c>
+      <c r="C10" s="2">
         <v>-1.01</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D10" s="2">
         <v>2.29</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E10" s="2">
         <v>-0.09</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F10" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>43113</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
+        <v>2.95</v>
+      </c>
+      <c r="C11" s="2">
         <v>-0.66</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D11" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E11" s="2">
         <v>-1.43</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F11" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>43112</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B12" s="2">
+        <v>-3.84</v>
+      </c>
+      <c r="C12" s="2">
         <v>2.38</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D12" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E12" s="2">
         <v>-3.52</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F12" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="13" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>43111</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B13" s="2">
+        <v>-8.33</v>
+      </c>
+      <c r="C13" s="2">
         <v>-4.13</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D13" s="2">
         <v>-4.57</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E13" s="2">
         <v>0.31</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F13" s="2">
         <v>-1.06</v>
       </c>
     </row>
-    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>43110</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B14" s="2">
+        <v>-6.81</v>
+      </c>
+      <c r="C14" s="2">
         <v>-3.96</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D14" s="2">
         <v>-2.85</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E14" s="2">
         <v>2.44</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F14" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="15" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>43109</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B15" s="2">
+        <v>-3.69</v>
+      </c>
+      <c r="C15" s="2">
         <v>-2.52</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D15" s="2">
         <v>-2.36</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E15" s="2">
         <v>-3.49</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F15" s="2">
         <v>-3.86</v>
       </c>
     </row>
-    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>43108</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B16" s="2">
+        <v>-1.91</v>
+      </c>
+      <c r="C16" s="2">
         <v>-3.15</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D16" s="2">
         <v>-3.31</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E16" s="2">
         <v>-2.99</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F16" s="2">
         <v>-5.51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>43107</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2.94</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3.32</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3.79</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>43106</v>
-      </c>
-      <c r="B15" s="2">
-        <v>9.02</v>
-      </c>
-      <c r="C15" s="2">
-        <v>9.2799999999999994</v>
-      </c>
-      <c r="D15" s="2">
-        <v>9.9600000000000009</v>
-      </c>
-      <c r="E15" s="2">
-        <v>9.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>43105</v>
-      </c>
-      <c r="B16" s="2">
-        <v>9.92</v>
-      </c>
-      <c r="C16" s="2">
-        <v>10.26</v>
-      </c>
-      <c r="D16" s="2">
-        <v>10.46</v>
-      </c>
-      <c r="E16" s="2">
-        <v>10.94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>43104</v>
       </c>
       <c r="B17" s="2">
         <f>SUM(B2:B16)</f>
+        <v>14.710000000000004</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.94</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.32</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3.79</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>43106</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
+        <v>9.02</v>
+      </c>
+      <c r="D18" s="2">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>43105</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
+        <v>9.92</v>
+      </c>
+      <c r="D19" s="2">
+        <v>10.26</v>
+      </c>
+      <c r="E19" s="2">
+        <v>10.46</v>
+      </c>
+      <c r="F19" s="2">
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>43104</v>
+      </c>
+      <c r="C20" s="2">
+        <f>SUM(C5:C19)</f>
         <v>-27.14</v>
       </c>
-      <c r="C17" s="2">
-        <f>SUM(C2:C16)</f>
+      <c r="D20" s="2">
+        <f>SUM(D5:D19)</f>
         <v>2.7300000000000004</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E20" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F20" s="2">
         <v>10.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>43103</v>
       </c>
-      <c r="D18" s="2">
-        <f>SUM(D3:D17)</f>
+      <c r="E21" s="2">
+        <f>SUM(E6:E20)</f>
         <v>-2.9999999999997584E-2</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F21" s="2">
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="2">
-        <f>SUM(E4:E18)</f>
+    <row r="22" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="2">
+        <f>SUM(F7:F21)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4:E18">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F7:F21">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="10" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D17">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="E6:E20">
+    <cfRule type="cellIs" dxfId="49" priority="7" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="D5:D19">
+    <cfRule type="cellIs" dxfId="47" priority="5" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="C5:C19">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B16 B18:B19">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1093,209 +1376,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>43113</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.19</v>
-      </c>
+        <v>43116</v>
+      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
+        <v>43115</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>43114</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>43113</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>43112</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
         <v>-1.76</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D6" s="2">
         <v>-3.11</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>43111</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
         <v>-5.31</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D7" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E7" s="2">
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>43110</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
         <v>-1.89</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D8" s="2">
         <v>4.54</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E8" s="2">
         <v>-1.19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>43109</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2">
         <v>-1.65</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D9" s="2">
         <v>0.2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E9" s="2">
         <v>-3.22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>43108</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B10" s="2">
+        <v>-1.71</v>
+      </c>
+      <c r="C10" s="2">
         <v>-1.07</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D10" s="2">
         <v>0.27</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E10" s="2">
         <v>-4.05</v>
       </c>
     </row>
-    <row r="8" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>43107</v>
-      </c>
-      <c r="B8" s="2">
-        <v>6.26</v>
-      </c>
-      <c r="C8" s="2">
-        <v>5.21</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3.07</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
-        <v>43106</v>
-      </c>
-      <c r="B9" s="2">
-        <v>12.27</v>
-      </c>
-      <c r="C9" s="2">
-        <v>12.63</v>
-      </c>
-      <c r="D9" s="2">
-        <v>11.89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>43105</v>
-      </c>
-      <c r="B10" s="2">
-        <v>12.23</v>
-      </c>
-      <c r="C10" s="2">
-        <v>13.07</v>
-      </c>
-      <c r="D10" s="2">
-        <v>13.07</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>43104</v>
       </c>
       <c r="B11" s="2">
         <f>SUM(B2:B10)</f>
+        <v>-1.71</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5.21</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>43106</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
+        <v>12.27</v>
+      </c>
+      <c r="D12" s="2">
+        <v>12.63</v>
+      </c>
+      <c r="E12" s="2">
+        <v>11.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>43105</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
+        <v>12.23</v>
+      </c>
+      <c r="D13" s="2">
+        <v>13.07</v>
+      </c>
+      <c r="E13" s="2">
+        <v>13.07</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>43104</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
+        <f>SUM(C5:C13)</f>
         <v>20.27</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D14" s="2">
         <v>11.69</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E14" s="2">
         <v>11.52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>43103</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="2">
-        <f>SUM(C3:C11)</f>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="2">
+        <f>SUM(D6:D14)</f>
         <v>47.05</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E15" s="2">
         <v>10.27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2">
-        <f>SUM(D4:D12)</f>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2">
+        <f>SUM(E7:E15)</f>
         <v>38.85</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D4:D12">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="E7:E15">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="D6:D14">
+    <cfRule type="cellIs" dxfId="39" priority="7" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C13">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:B14">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1306,416 +1653,525 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
+        <v>43121</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-6.17</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>43120</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-8.44</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>43119</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-9.1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>43118</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B5" s="2">
+        <v>-9.01</v>
+      </c>
+      <c r="C5" s="2">
         <v>-7.22</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>43117</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B6" s="2">
+        <v>-1.77</v>
+      </c>
+      <c r="C6" s="2">
         <v>-4.34</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D6" s="2">
         <v>-5.25</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="E6" s="2"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>43116</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B7" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="C7" s="2">
         <v>-0.59</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D7" s="2">
         <v>-2.1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E7" s="2">
         <v>-3.32</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F7" s="2">
         <v>-0.98</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G7" s="2">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>43115</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="C8" s="2">
         <v>2.73</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D8" s="2">
         <v>1.07</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E8" s="2">
         <v>0.05</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F8" s="2">
         <v>1.6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G8" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="9" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>43114</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B9" s="2">
+        <v>8.39</v>
+      </c>
+      <c r="C9" s="2">
         <v>4.32</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D9" s="2">
         <v>3.59</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E9" s="2">
         <v>2.62</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F9" s="2">
         <v>3.37</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G9" s="2">
         <v>4.62</v>
       </c>
     </row>
-    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="10" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>43113</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B10" s="2">
+        <v>2.16</v>
+      </c>
+      <c r="C10" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D10" s="2">
         <v>3.63</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E10" s="2">
         <v>2.06</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F10" s="2">
         <v>2.59</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G10" s="2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="11" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>43112</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
+        <v>-4.3099999999999996</v>
+      </c>
+      <c r="C11" s="2">
         <v>-0.08</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D11" s="2">
         <v>0.46</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E11" s="2">
         <v>1.44</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F11" s="2">
         <v>1.58</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G11" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="12" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>43111</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B12" s="2">
+        <v>-7.86</v>
+      </c>
+      <c r="C12" s="2">
         <v>-5.05</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D12" s="2">
         <v>-3.31</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E12" s="2">
         <v>2.34</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F12" s="2">
         <v>0.63</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G12" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="13" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>43110</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B13" s="2">
+        <v>-4.5</v>
+      </c>
+      <c r="C13" s="2">
         <v>-3.68</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D13" s="2">
         <v>-2.74</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E13" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F13" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G13" s="2">
         <v>1.63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="14" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>43109</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B14" s="2">
+        <v>-2.31</v>
+      </c>
+      <c r="C14" s="2">
         <v>-2.34</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D14" s="2">
         <v>-1.72</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E14" s="2">
         <v>-0.82</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F14" s="2">
         <v>-0.25</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G14" s="2">
         <v>-1.66</v>
       </c>
     </row>
-    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="15" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>43108</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B15" s="2">
+        <v>-1.3</v>
+      </c>
+      <c r="C15" s="2">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D15" s="2">
         <v>-0.92</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E15" s="2">
         <v>-0.84</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F15" s="2">
         <v>-1.61</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G15" s="2">
         <v>-3.16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="16" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>43107</v>
-      </c>
-      <c r="B13" s="2">
-        <v>6.29</v>
-      </c>
-      <c r="C13" s="2">
-        <v>6.25</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5.26</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3.76</v>
-      </c>
-      <c r="F13" s="2">
-        <v>2.85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>43106</v>
-      </c>
-      <c r="B14" s="2">
-        <v>12.56</v>
-      </c>
-      <c r="C14" s="2">
-        <v>12.6</v>
-      </c>
-      <c r="D14" s="2">
-        <v>13.02</v>
-      </c>
-      <c r="E14" s="2">
-        <v>12.61</v>
-      </c>
-      <c r="F14" s="2">
-        <v>12.42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>43105</v>
-      </c>
-      <c r="B15" s="2">
-        <v>12.51</v>
-      </c>
-      <c r="C15" s="2">
-        <v>12.64</v>
-      </c>
-      <c r="D15" s="2">
-        <v>13.24</v>
-      </c>
-      <c r="E15" s="2">
-        <v>13.38</v>
-      </c>
-      <c r="F15" s="2">
-        <v>13.55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>43104</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
+        <v>-32.53</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6.29</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6.25</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5.26</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3.76</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>43106</v>
+      </c>
+      <c r="C17" s="2">
+        <v>12.56</v>
+      </c>
+      <c r="D17" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>13.02</v>
+      </c>
+      <c r="F17" s="2">
+        <v>12.61</v>
+      </c>
+      <c r="G17" s="2">
+        <v>12.42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>43105</v>
+      </c>
+      <c r="C18" s="2">
+        <v>12.51</v>
+      </c>
+      <c r="D18" s="2">
+        <v>12.64</v>
+      </c>
+      <c r="E18" s="2">
+        <v>13.24</v>
+      </c>
+      <c r="F18" s="2">
+        <v>13.38</v>
+      </c>
+      <c r="G18" s="2">
+        <v>13.55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>43104</v>
+      </c>
+      <c r="C19" s="2">
+        <f>SUM(C5:C18)</f>
         <v>16.470000000000002</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D19" s="2">
         <v>11.71</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E19" s="2">
         <v>11.91</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F19" s="2">
         <v>11.84</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G19" s="2">
         <v>11.9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="20" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>43103</v>
       </c>
-      <c r="C17" s="2">
-        <f>SUM(C3:C16)</f>
+      <c r="D20" s="2">
+        <f>SUM(D6:D19)</f>
         <v>35.909999999999997</v>
       </c>
-      <c r="D17" s="2">
-        <f>SUM(D3:D16)</f>
+      <c r="E20" s="2">
+        <f>SUM(E6:E19)</f>
         <v>49.22</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F20" s="2">
         <v>10.97</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G20" s="2">
         <v>10.72</v>
       </c>
     </row>
-    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="2">
-        <f>SUM(E4:E17)</f>
+    <row r="21" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="2">
+        <f>SUM(F7:F20)</f>
         <v>60.58</v>
       </c>
-      <c r="F18" s="2">
-        <f>SUM(F4:F17)</f>
+      <c r="G21" s="2">
+        <f>SUM(G7:G20)</f>
         <v>59.83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="E4:F17">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F7:G20">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E17">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F7:F20">
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="E6:E19">
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="E6:E19">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C16">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="D6:D19">
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C16">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="D6:D19">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="C9:C18">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="C9:C18">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C8">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C8">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B15">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B15">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update GFS on 201801090027
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">2018-01-08 12z </t>
+  </si>
+  <si>
+    <t>2018-01-09 00z</t>
   </si>
 </sst>
 </file>
@@ -141,92 +144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1022,517 +940,577 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>43123</v>
       </c>
       <c r="B2" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="C2" s="2">
         <v>-0.26</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>43122</v>
       </c>
       <c r="B3" s="2">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="C3" s="2">
         <v>4.21</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>1.91</v>
       </c>
-      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43121</v>
       </c>
       <c r="B4" s="2">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="C4" s="2">
         <v>2.71</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>-0.15</v>
       </c>
-      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>43120</v>
       </c>
       <c r="B5" s="2">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="C5" s="2">
         <v>-4.7300000000000004</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>-0.85</v>
       </c>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>43119</v>
       </c>
       <c r="B6" s="2">
+        <v>-5.59</v>
+      </c>
+      <c r="C6" s="2">
         <v>-7.41</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>3.11</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>-10.98</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>-10.28</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>43118</v>
       </c>
       <c r="B7" s="2">
+        <v>-2.06</v>
+      </c>
+      <c r="C7" s="2">
         <v>-8.9499999999999993</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>6.76</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>-10.48</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>-6.81</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>43117</v>
       </c>
       <c r="B8" s="2">
+        <v>6.01</v>
+      </c>
+      <c r="C8" s="2">
         <v>-8.8699999999999992</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>1.81</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>-8.9</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>-0.99</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>43116</v>
       </c>
       <c r="B9" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="C9" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>4.46</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>3.95</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>-6.26</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>43115</v>
       </c>
       <c r="B10" s="2">
+        <v>6.24</v>
+      </c>
+      <c r="C10" s="2">
         <v>6.49</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>9.85</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>-1.5</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>43114</v>
       </c>
       <c r="B11" s="2">
+        <v>6.74</v>
+      </c>
+      <c r="C11" s="2">
         <v>9.66</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>9.44</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>-1.01</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>2.29</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>-0.09</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>43113</v>
       </c>
       <c r="B12" s="2">
+        <v>2.66</v>
+      </c>
+      <c r="C12" s="2">
         <v>4.0599999999999996</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>2.95</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>-0.66</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>-1.43</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>43112</v>
       </c>
       <c r="B13" s="2">
+        <v>-3.93</v>
+      </c>
+      <c r="C13" s="2">
         <v>-3.42</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>-3.84</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>2.38</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>-3.52</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43111</v>
       </c>
       <c r="B14" s="2">
+        <v>-8.61</v>
+      </c>
+      <c r="C14" s="2">
         <v>-8.68</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>-8.33</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>-4.13</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>-4.57</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.31</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>-1.06</v>
       </c>
     </row>
-    <row r="15" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43110</v>
       </c>
       <c r="B15" s="2">
+        <v>-6.92</v>
+      </c>
+      <c r="C15" s="2">
         <v>-7.18</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>-6.81</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>-3.96</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>-2.85</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>2.44</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="16" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>43109</v>
       </c>
       <c r="B16" s="2">
+        <v>-4.1500000000000004</v>
+      </c>
+      <c r="C16" s="2">
         <v>-3.79</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>-3.69</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>-2.52</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>-2.36</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>-3.49</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>-3.86</v>
       </c>
     </row>
-    <row r="17" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>43108</v>
       </c>
       <c r="B17">
         <f>SUM(B2:B16)</f>
+        <v>1.1999999999999993</v>
+      </c>
+      <c r="C17">
+        <f>SUM(C2:C16)</f>
         <v>-28.169999999999991</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>-1.91</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>-3.15</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>-3.31</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>-2.99</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>-5.51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>43107</v>
       </c>
-      <c r="C18">
-        <f>SUM(C3:C17)</f>
+      <c r="D18">
+        <f>SUM(D3:D17)</f>
         <v>14.710000000000004</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>2.94</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>3.32</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>3.79</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>43106</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>9.02</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>9.2799999999999994</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>9.9600000000000009</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>9.36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>43105</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <v>9.92</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>10.26</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>10.46</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>10.94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>43104</v>
       </c>
-      <c r="D21">
-        <f>SUM(D6:D20)</f>
-        <v>-27.14</v>
-      </c>
       <c r="E21">
         <f>SUM(E6:E20)</f>
+        <v>-27.14</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F6:F20)</f>
         <v>2.7300000000000004</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>10.3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>43103</v>
       </c>
-      <c r="F22" s="2">
-        <f>SUM(F7:F21)</f>
+      <c r="G22" s="2">
+        <f>SUM(G7:G21)</f>
         <v>-2.9999999999997584E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="23" spans="1:7" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G23" s="2">
-        <f>SUM(G8:G22)</f>
+    <row r="23" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="2">
+        <f>SUM(H8:H22)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G8:G22">
-    <cfRule type="cellIs" dxfId="57" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="16" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F21">
-    <cfRule type="cellIs" dxfId="55" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="14" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H8:H22">
+    <cfRule type="cellIs" dxfId="55" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="18" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G21">
+    <cfRule type="cellIs" dxfId="53" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F20">
+    <cfRule type="cellIs" dxfId="51" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:E20">
-    <cfRule type="cellIs" dxfId="53" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D20">
-    <cfRule type="cellIs" dxfId="51" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C17 C19:C20">
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:E16 B19:E20 C17:E17 B18 D18:E18 B22:E1048576 B21:C21">
-    <cfRule type="cellIs" dxfId="47" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="6" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B22">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:B22">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D17 D19:D20">
+    <cfRule type="cellIs" dxfId="47" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:F16 C19:F20 D17:F17 C18 E18:F18 C22:F1048576 C21:D21">
+    <cfRule type="cellIs" dxfId="45" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C22">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C22">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B16">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1549,14 +1527,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -1571,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43117</v>
       </c>
@@ -1582,7 +1560,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43116</v>
       </c>
@@ -1593,7 +1571,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43115</v>
       </c>
@@ -1604,7 +1582,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43114</v>
       </c>
@@ -1615,7 +1593,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43113</v>
       </c>
@@ -1628,7 +1606,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43112</v>
       </c>
@@ -1643,7 +1621,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43111</v>
       </c>
@@ -1660,7 +1638,7 @@
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43110</v>
       </c>
@@ -1677,7 +1655,7 @@
         <v>-1.19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43109</v>
       </c>
@@ -1694,7 +1672,7 @@
         <v>-3.22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43108</v>
       </c>
@@ -1712,7 +1690,7 @@
         <v>-4.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43107</v>
       </c>
@@ -1726,7 +1704,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43106</v>
       </c>
@@ -1741,7 +1719,7 @@
         <v>11.89</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43105</v>
       </c>
@@ -1756,7 +1734,7 @@
         <v>13.07</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43104</v>
       </c>
@@ -1772,7 +1750,7 @@
         <v>11.52</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43103</v>
       </c>
@@ -1786,7 +1764,7 @@
         <v>10.27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1798,42 +1776,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E8:E16">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D15">
-    <cfRule type="cellIs" dxfId="39" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:C14">
-    <cfRule type="cellIs" dxfId="37" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B10">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1847,22 +1825,22 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1885,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43122</v>
       </c>
@@ -1898,7 +1876,7 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43121</v>
       </c>
@@ -1913,7 +1891,7 @@
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43120</v>
       </c>
@@ -1928,7 +1906,7 @@
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43119</v>
       </c>
@@ -1943,7 +1921,7 @@
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43118</v>
       </c>
@@ -1960,7 +1938,7 @@
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43117</v>
       </c>
@@ -1979,7 +1957,7 @@
       <c r="F7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43116</v>
       </c>
@@ -2005,12 +1983,12 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>43115</v>
       </c>
       <c r="B9" s="2">
-        <v>8.17</v>
+        <v>8.14</v>
       </c>
       <c r="C9" s="2">
         <v>7.99</v>
@@ -2031,7 +2009,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43114</v>
       </c>
@@ -2057,7 +2035,7 @@
         <v>4.62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>43113</v>
       </c>
@@ -2083,7 +2061,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43112</v>
       </c>
@@ -2109,7 +2087,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>43111</v>
       </c>
@@ -2135,7 +2113,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43110</v>
       </c>
@@ -2161,7 +2139,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>43109</v>
       </c>
@@ -2187,13 +2165,13 @@
         <v>-1.66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43108</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
-        <v>-28.79</v>
+        <v>-28.82</v>
       </c>
       <c r="C16" s="2">
         <v>-1.3</v>
@@ -2214,7 +2192,7 @@
         <v>-3.16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>43107</v>
       </c>
@@ -2238,7 +2216,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>43106</v>
       </c>
@@ -2258,7 +2236,7 @@
         <v>12.42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>43105</v>
       </c>
@@ -2278,7 +2256,7 @@
         <v>13.55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>43104</v>
       </c>
@@ -2299,7 +2277,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>43103</v>
       </c>
@@ -2318,7 +2296,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G22" s="2">
         <f>SUM(G8:G21)</f>
         <v>60.58</v>
@@ -2328,117 +2306,117 @@
         <v>59.83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="G8:H21">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G21">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F20">
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F20">
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E20">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E20">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D19">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D19">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D9">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D9">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C16">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C16">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update GFS on 201801091158
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>2018-01-09 00z</t>
+  </si>
+  <si>
+    <t> 2018-01-09 12z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01-09 00z </t>
   </si>
 </sst>
 </file>
@@ -144,7 +150,143 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -940,577 +1082,650 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43123</v>
+        <v>43124</v>
       </c>
       <c r="B2" s="2">
-        <v>3.69</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-0.26</v>
-      </c>
+        <v>5.57</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
+        <v>43123</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6.14</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>43122</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="C4" s="2">
         <v>4.8899999999999997</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D4" s="2">
         <v>4.21</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E4" s="2">
         <v>1.91</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>43121</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
+        <v>-6.26</v>
+      </c>
+      <c r="C5" s="2">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="2">
         <v>2.71</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E5" s="2">
         <v>-0.15</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43120</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>-9.06</v>
+      </c>
+      <c r="C6" s="2">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>-4.7300000000000004</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>-0.85</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43119</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>-5.84</v>
+      </c>
+      <c r="C7" s="2">
         <v>-5.59</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>-7.41</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>3.11</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>-10.98</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G7" s="2">
         <v>-10.28</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43118</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C8" s="2">
         <v>-2.06</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>-8.9499999999999993</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>6.76</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>-10.48</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>-6.81</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H8" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43117</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>7.69</v>
+      </c>
+      <c r="C9" s="2">
         <v>6.01</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>-8.8699999999999992</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>1.81</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>-8.9</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-0.99</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="10" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43116</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="C10" s="2">
         <v>7.9</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>4.46</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>3.95</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>-6.26</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="11" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43115</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>5.91</v>
+      </c>
+      <c r="C11" s="2">
         <v>6.24</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>6.49</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>9.85</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>-1.5</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="12" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>43114</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>7.16</v>
+      </c>
+      <c r="C12" s="2">
         <v>6.74</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>9.66</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>9.44</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>-1.01</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>2.29</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>-0.09</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="13" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43113</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C13" s="2">
         <v>2.66</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>4.0599999999999996</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>2.95</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>-0.66</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>-1.43</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="14" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43112</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
+        <v>-4.38</v>
+      </c>
+      <c r="C14" s="2">
         <v>-3.93</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="2">
         <v>-3.42</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>-3.84</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>2.38</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>-3.52</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="15" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43111</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>-8.7799999999999994</v>
+      </c>
+      <c r="C15" s="2">
         <v>-8.61</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>-8.68</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>-8.33</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>-4.13</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>-4.57</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>0.31</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <v>-1.06</v>
       </c>
     </row>
-    <row r="15" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="16" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43110</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="2">
+        <v>-6.68</v>
+      </c>
+      <c r="C16" s="2">
         <v>-6.92</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D16" s="2">
         <v>-7.18</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E16" s="2">
         <v>-6.81</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F16" s="2">
         <v>-3.96</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G16" s="2">
         <v>-2.85</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H16" s="2">
         <v>2.44</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I16" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="17" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
         <v>43109</v>
-      </c>
-      <c r="B16" s="2">
-        <v>-4.1500000000000004</v>
-      </c>
-      <c r="C16" s="2">
-        <v>-3.79</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-3.69</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-2.52</v>
-      </c>
-      <c r="F16" s="2">
-        <v>-2.36</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-3.49</v>
-      </c>
-      <c r="H16" s="2">
-        <v>-3.86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>43108</v>
       </c>
       <c r="B17">
         <f>SUM(B2:B16)</f>
+        <v>4.1200000000000028</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-4.1500000000000004</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-3.79</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-3.69</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-2.52</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-2.36</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-3.49</v>
+      </c>
+      <c r="I17" s="2">
+        <v>-3.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>43108</v>
+      </c>
+      <c r="C18">
+        <f>SUM(C3:C17)</f>
         <v>1.1999999999999993</v>
-      </c>
-      <c r="C17">
-        <f>SUM(C2:C16)</f>
-        <v>-28.169999999999991</v>
-      </c>
-      <c r="D17" s="2">
-        <v>-1.91</v>
-      </c>
-      <c r="E17" s="2">
-        <v>-3.15</v>
-      </c>
-      <c r="F17" s="2">
-        <v>-3.31</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-2.99</v>
-      </c>
-      <c r="H17" s="2">
-        <v>-5.51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>43107</v>
       </c>
       <c r="D18">
         <f>SUM(D3:D17)</f>
+        <v>-28.169999999999991</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-1.91</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-3.15</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-3.31</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-2.99</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-5.51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>43107</v>
+      </c>
+      <c r="E19">
+        <f>SUM(E4:E18)</f>
         <v>14.710000000000004</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F19" s="2">
         <v>2.94</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G19" s="2">
         <v>3.32</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H19" s="2">
         <v>3.79</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I19" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="20" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
         <v>43106</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F20" s="2">
         <v>9.02</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G20" s="2">
         <v>9.2799999999999994</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H20" s="2">
         <v>9.9600000000000009</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I20" s="2">
         <v>9.36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="21" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
         <v>43105</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F21" s="2">
         <v>9.92</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G21" s="2">
         <v>10.26</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H21" s="2">
         <v>10.46</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I21" s="2">
         <v>10.94</v>
       </c>
     </row>
-    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
         <v>43104</v>
       </c>
-      <c r="E21">
-        <f>SUM(E6:E20)</f>
+      <c r="F22">
+        <f>SUM(F7:F21)</f>
         <v>-27.14</v>
       </c>
-      <c r="F21">
-        <f>SUM(F6:F20)</f>
+      <c r="G22">
+        <f>SUM(G7:G21)</f>
         <v>2.7300000000000004</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H22" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I22" s="2">
         <v>10.3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+    <row r="23" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
         <v>43103</v>
       </c>
-      <c r="G22" s="2">
-        <f>SUM(G7:G21)</f>
-        <v>-2.9999999999997584E-2</v>
-      </c>
-      <c r="H22" s="2">
-        <v>9.6300000000000008</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H23" s="2">
         <f>SUM(H8:H22)</f>
+        <v>-2.9999999999997584E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="2">
+        <f>SUM(I9:I23)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I9:I23">
+    <cfRule type="cellIs" dxfId="67" priority="19" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H8:H22">
-    <cfRule type="cellIs" dxfId="55" priority="17" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="18" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G21">
-    <cfRule type="cellIs" dxfId="53" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F20">
-    <cfRule type="cellIs" dxfId="51" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="14" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6:E20">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D17 D19:D20">
-    <cfRule type="cellIs" dxfId="47" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F16 C19:F20 D17:F17 C18 E18:F18 C22:F1048576 C21:D21">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C22">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C22">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:F21">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="14" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E18 E20:E21">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:G17 D20:G21 E18:G18 D19 F19:G19 D23:G1048576 D22:E22">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:D23">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19:D23">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C17">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1521,124 +1736,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43117</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="C2" s="1">
         <v>0.89</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43116</v>
       </c>
       <c r="B3" s="2">
+        <v>5.74</v>
+      </c>
+      <c r="C3" s="2">
         <v>7.57</v>
       </c>
-      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43115</v>
       </c>
       <c r="B4" s="2">
+        <v>7.93</v>
+      </c>
+      <c r="C4" s="2">
         <v>9.86</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43114</v>
       </c>
       <c r="B5" s="2">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="C5" s="2">
         <v>9.44</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43113</v>
       </c>
       <c r="B6" s="2">
+        <v>2.97</v>
+      </c>
+      <c r="C6" s="2">
         <v>2.96</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>1.19</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43112</v>
       </c>
       <c r="B7" s="2">
+        <v>-4.29</v>
+      </c>
+      <c r="C7" s="2">
         <v>-4.58</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>-1.76</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>-3.11</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43111</v>
       </c>
       <c r="B8" s="2">
+        <v>-8.25</v>
+      </c>
+      <c r="C8" s="2">
         <v>-8.76</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>-5.31</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43110</v>
       </c>
@@ -1646,172 +1885,196 @@
         <v>-5.99</v>
       </c>
       <c r="C9" s="2">
+        <v>-5.99</v>
+      </c>
+      <c r="D9" s="2">
         <v>-1.89</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>4.54</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>-1.19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43109</v>
       </c>
       <c r="B10" s="2">
+        <v>-3.68</v>
+      </c>
+      <c r="C10" s="2">
         <v>-3.28</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>-1.65</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>0.2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>-3.22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43108</v>
       </c>
       <c r="B11" s="2">
         <f>SUM(B2:B10)</f>
+        <v>6.24</v>
+      </c>
+      <c r="C11" s="2">
+        <f>SUM(C2:C10)</f>
         <v>8.110000000000003</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>-1.07</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>0.27</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>-4.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43107</v>
       </c>
-      <c r="C12" s="2">
+      <c r="B12" s="6"/>
+      <c r="D12" s="2">
         <v>6.26</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>5.21</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>3.07</v>
       </c>
     </row>
-    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43106</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>12.27</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>12.63</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>11.89</v>
       </c>
     </row>
-    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43105</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>12.23</v>
-      </c>
-      <c r="D14" s="2">
-        <v>13.07</v>
       </c>
       <c r="E14" s="2">
         <v>13.07</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="2">
+        <v>13.07</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43104</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <f>SUM(C6:C14)</f>
+      <c r="B15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <f>SUM(D6:D14)</f>
         <v>20.27</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>11.69</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>11.52</v>
       </c>
     </row>
-    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43103</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="2">
-        <f>SUM(D7:D15)</f>
+      <c r="D16" s="6"/>
+      <c r="E16" s="2">
+        <f>SUM(E7:E15)</f>
         <v>47.05</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>10.27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="2">
-        <f>SUM(E8:E16)</f>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2">
+        <f>SUM(F8:F16)</f>
         <v>38.85</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E8:E16">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D15">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C14">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B15">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B10">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="F8:F16">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E15">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D14">
+    <cfRule type="cellIs" dxfId="43" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C15">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B10">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1822,601 +2085,666 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>43122</v>
       </c>
       <c r="B2" s="2">
+        <v>-2.93</v>
+      </c>
+      <c r="C2" s="2">
         <v>-4.07</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43121</v>
       </c>
       <c r="B3" s="2">
+        <v>-5.67</v>
+      </c>
+      <c r="C3" s="2">
         <v>-6.47</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>-6.17</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43120</v>
       </c>
       <c r="B4" s="2">
+        <v>-8.2200000000000006</v>
+      </c>
+      <c r="C4" s="2">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>-8.44</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
       <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43119</v>
       </c>
       <c r="B5" s="2">
+        <v>-7.44</v>
+      </c>
+      <c r="C5" s="2">
         <v>-9.09</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>-9.1</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>43118</v>
       </c>
       <c r="B6" s="2">
+        <v>-1.7</v>
+      </c>
+      <c r="C6" s="2">
         <v>-4.87</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>-9.01</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>-7.22</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>43117</v>
       </c>
       <c r="B7" s="2">
+        <v>4.28</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>-1.77</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>-4.34</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>-5.25</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="2"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>43116</v>
       </c>
       <c r="B8" s="2">
+        <v>7.11</v>
+      </c>
+      <c r="C8" s="2">
         <v>5.13</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>3.7</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>-0.59</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>-2.1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>-3.32</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>-0.98</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>43115</v>
       </c>
       <c r="B9" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="C9" s="2">
         <v>8.14</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>7.99</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>2.73</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>1.07</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0.05</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>1.6</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43114</v>
       </c>
       <c r="B10" s="2">
+        <v>9.26</v>
+      </c>
+      <c r="C10" s="2">
         <v>8.92</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>8.39</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>4.32</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>3.59</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>2.62</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>3.37</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>4.62</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>43113</v>
       </c>
       <c r="B11" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="C11" s="2">
         <v>3.02</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>2.16</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>3.63</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>2.06</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>2.59</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>43112</v>
       </c>
       <c r="B12" s="2">
+        <v>-4</v>
+      </c>
+      <c r="C12" s="2">
         <v>-3.95</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>-4.3099999999999996</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>-0.08</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>0.46</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>1.44</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>1.58</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>43111</v>
       </c>
       <c r="B13" s="2">
+        <v>-8.1300000000000008</v>
+      </c>
+      <c r="C13" s="2">
         <v>-8.5299999999999994</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>-7.86</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>-5.05</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>-3.31</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>2.34</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>0.63</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>43110</v>
       </c>
       <c r="B14" s="2">
+        <v>-5.58</v>
+      </c>
+      <c r="C14" s="2">
         <v>-5.64</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>-4.5</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>-3.68</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>-2.74</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>1.63</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>43109</v>
       </c>
       <c r="B15" s="2">
+        <v>-3.51</v>
+      </c>
+      <c r="C15" s="2">
         <v>-3.11</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>-2.31</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>-2.34</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>-1.72</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>-0.82</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>-0.25</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>-1.66</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43108</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
+        <v>-15.48</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUM(C2:C15)</f>
         <v>-28.82</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>-1.3</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>-0.92</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>-0.84</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>-1.61</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>-3.16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>43107</v>
       </c>
-      <c r="C17" s="2">
-        <f>SUM(C3:C16)</f>
+      <c r="D17" s="2">
+        <f>SUM(D3:D16)</f>
         <v>-32.53</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>6.29</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>6.25</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>5.26</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>3.76</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>2.85</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>43106</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>12.56</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>12.6</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>13.02</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>12.61</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>12.42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>43105</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>12.51</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>12.64</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>13.24</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>13.38</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>13.55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>43104</v>
       </c>
-      <c r="D20" s="2">
-        <f>SUM(D6:D19)</f>
+      <c r="E20" s="2">
+        <f>SUM(E6:E19)</f>
         <v>16.470000000000002</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>11.71</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>11.91</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>11.84</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>11.9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>43103</v>
       </c>
-      <c r="E21" s="2">
-        <f>SUM(E7:E20)</f>
-        <v>35.909999999999997</v>
-      </c>
       <c r="F21" s="2">
         <f>SUM(F7:F20)</f>
+        <v>35.909999999999997</v>
+      </c>
+      <c r="G21" s="2">
+        <f>SUM(G7:G20)</f>
         <v>49.22</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>10.97</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>10.72</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="2">
-        <f>SUM(G8:G21)</f>
-        <v>60.58</v>
-      </c>
+    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H22" s="2">
         <f>SUM(H8:H21)</f>
+        <v>60.58</v>
+      </c>
+      <c r="I22" s="2">
+        <f>SUM(I8:I21)</f>
         <v>59.83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="G8:H21">
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G21">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="H8:I21">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H21">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="30" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G20">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="28" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G20">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F20">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F20">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E20">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E20">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D19">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D19">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D9">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:D9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C16">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:C16">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E19">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E19">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:E9">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:E9">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D16">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D16">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C15">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C15">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update GFS data on 201801101226
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -59,6 +59,12 @@
   <si>
     <t xml:space="preserve">2018-01-09 00z </t>
   </si>
+  <si>
+    <t>2018-01-10 12z</t>
+  </si>
+  <si>
+    <t>2018-01-10 00z</t>
+  </si>
 </sst>
 </file>
 
@@ -67,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +97,21 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -134,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -146,11 +167,68 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1082,56 +1160,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="E17:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43124</v>
+        <v>43125</v>
       </c>
       <c r="B2" s="2">
-        <v>5.57</v>
+        <v>-6.08</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1140,592 +1222,684 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43123</v>
+        <v>43124</v>
       </c>
       <c r="B3" s="2">
-        <v>6.14</v>
+        <v>-1.9</v>
       </c>
       <c r="C3" s="2">
-        <v>3.69</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-0.26</v>
-      </c>
+        <v>5.57</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
+        <v>43123</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-0.34</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.14</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>43122</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
+        <v>-3.93</v>
+      </c>
+      <c r="C5" s="2">
         <v>2.0299999999999998</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="2">
         <v>4.8899999999999997</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E5" s="2">
         <v>4.21</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F5" s="2">
         <v>1.91</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43121</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>-8.11</v>
+      </c>
+      <c r="C6" s="2">
         <v>-6.26</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>2.71</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F6" s="2">
         <v>-0.15</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43120</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>-10.65</v>
+      </c>
+      <c r="C7" s="2">
         <v>-9.06</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>-4.7300000000000004</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>-0.85</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43119</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>-8.5500000000000007</v>
+      </c>
+      <c r="C8" s="2">
         <v>-5.84</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>-5.59</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>-7.41</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>3.11</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>-10.98</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H8" s="2">
         <v>-10.28</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43118</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>-1.61</v>
+      </c>
+      <c r="C9" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>-2.06</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>-8.9499999999999993</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>6.76</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-10.48</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-6.81</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43117</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="C10" s="2">
         <v>7.69</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>6.01</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>-8.8699999999999992</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>1.81</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>-8.9</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>-0.99</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J10" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+    <row r="11" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43116</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>6.75</v>
+      </c>
+      <c r="C11" s="2">
         <v>7.21</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>7.9</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>4.46</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>3.95</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <v>-6.26</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J11" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="11" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>43115</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>5.03</v>
+      </c>
+      <c r="C12" s="2">
         <v>5.91</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>6.24</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>6.49</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>9.85</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>-1.5</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J12" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43114</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="C13" s="2">
         <v>7.16</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>6.74</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>9.66</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>9.44</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>-1.01</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>2.29</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <v>-0.09</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J13" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43113</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
+        <v>2.48</v>
+      </c>
+      <c r="C14" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="2">
         <v>2.66</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>4.0599999999999996</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>2.95</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>-0.66</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <v>-1.43</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J14" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="14" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43112</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>-4.12</v>
+      </c>
+      <c r="C15" s="2">
         <v>-4.38</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>-3.93</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>-3.42</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>-3.84</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>2.38</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <v>-3.52</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J15" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="15" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43111</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="2">
+        <v>-9.23</v>
+      </c>
+      <c r="C16" s="2">
         <v>-8.7799999999999994</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D16" s="2">
         <v>-8.61</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E16" s="2">
         <v>-8.68</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F16" s="2">
         <v>-8.33</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G16" s="2">
         <v>-4.13</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H16" s="2">
         <v>-4.57</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I16" s="2">
         <v>0.31</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J16" s="2">
         <v>-1.06</v>
       </c>
     </row>
-    <row r="16" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+    <row r="17" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
         <v>43110</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="7">
+        <f>SUM(B2:B16)</f>
+        <v>-27.77</v>
+      </c>
+      <c r="C17" s="2">
         <v>-6.68</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D17" s="2">
         <v>-6.92</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E17" s="2">
         <v>-7.18</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F17" s="2">
         <v>-6.81</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G17" s="2">
         <v>-3.96</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H17" s="2">
         <v>-2.85</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I17" s="2">
         <v>2.44</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J17" s="2">
         <v>3.01</v>
       </c>
     </row>
-    <row r="17" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+    <row r="18" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
         <v>43109</v>
       </c>
-      <c r="B17">
-        <f>SUM(B2:B16)</f>
+      <c r="B18" s="8"/>
+      <c r="C18" s="7">
+        <f>SUM(C3:C17)</f>
         <v>4.1200000000000028</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D18" s="2">
         <v>-4.1500000000000004</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E18" s="2">
         <v>-3.79</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F18" s="2">
         <v>-3.69</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G18" s="2">
         <v>-2.52</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H18" s="2">
         <v>-2.36</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I18" s="2">
         <v>-3.49</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J18" s="2">
         <v>-3.86</v>
       </c>
     </row>
-    <row r="18" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    <row r="19" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
         <v>43108</v>
       </c>
-      <c r="C18">
-        <f>SUM(C3:C17)</f>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="7">
+        <f>SUM(D4:D18)</f>
         <v>1.1999999999999993</v>
       </c>
-      <c r="D18">
-        <f>SUM(D3:D17)</f>
+      <c r="E19" s="7">
+        <f>SUM(E4:E18)</f>
         <v>-28.169999999999991</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F19" s="2">
         <v>-1.91</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G19" s="2">
         <v>-3.15</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H19" s="2">
         <v>-3.31</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I19" s="2">
         <v>-2.99</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J19" s="2">
         <v>-5.51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    <row r="20" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
         <v>43107</v>
       </c>
-      <c r="E19">
-        <f>SUM(E4:E18)</f>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="F20" s="7">
+        <f>SUM(F5:F19)</f>
         <v>14.710000000000004</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G20" s="2">
         <v>2.94</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H20" s="2">
         <v>3.32</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I20" s="2">
         <v>3.79</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J20" s="2">
         <v>1.33</v>
       </c>
     </row>
-    <row r="20" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    <row r="21" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
         <v>43106</v>
       </c>
-      <c r="F20" s="2">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="G21" s="2">
         <v>9.02</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H21" s="2">
         <v>9.2799999999999994</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I21" s="2">
         <v>9.9600000000000009</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J21" s="2">
         <v>9.36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    <row r="22" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
         <v>43105</v>
       </c>
-      <c r="F21" s="2">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="G22" s="2">
         <v>9.92</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H22" s="2">
         <v>10.26</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I22" s="2">
         <v>10.46</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J22" s="2">
         <v>10.94</v>
       </c>
     </row>
-    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+    <row r="23" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
         <v>43104</v>
       </c>
-      <c r="F22">
-        <f>SUM(F7:F21)</f>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="G23" s="7">
+        <f>SUM(G8:G22)</f>
         <v>-27.14</v>
       </c>
-      <c r="G22">
-        <f>SUM(G7:G21)</f>
+      <c r="H23" s="7">
+        <f>SUM(H8:H22)</f>
         <v>2.7300000000000004</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I23" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J23" s="2">
         <v>10.3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+    <row r="24" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
         <v>43103</v>
       </c>
-      <c r="H23" s="2">
-        <f>SUM(H8:H22)</f>
-        <v>-2.9999999999997584E-2</v>
-      </c>
-      <c r="I23" s="2">
-        <v>9.6300000000000008</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
       <c r="I24" s="2">
         <f>SUM(I9:I23)</f>
+        <v>-2.9999999999997584E-2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="2">
+        <f>SUM(J10:J24)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J10:J24">
+    <cfRule type="cellIs" dxfId="75" priority="21" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="22" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I9:I23">
-    <cfRule type="cellIs" dxfId="67" priority="19" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="73" priority="19" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="20" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H22">
-    <cfRule type="cellIs" dxfId="65" priority="17" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="18" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G21">
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="16" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F21">
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E18 E20:E21">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:G17 D20:G21 E18:G18 D19 F19:G19 D23:G1048576 D22:E22">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D23">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19:D23">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="18" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G22">
+    <cfRule type="cellIs" dxfId="69" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F19 F21:F22">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="14" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:H18 E21:H22 F19:H19 E20 G20:H20 E24:H1048576 E23:F23">
+    <cfRule type="cellIs" dxfId="65" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E24">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:E24">
+    <cfRule type="cellIs" dxfId="61" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D18">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1736,345 +1910,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
+        <v>43118</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7.46</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>43117</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
+        <v>10.86</v>
+      </c>
+      <c r="C3" s="2">
         <v>1.76</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="9">
         <v>0.89</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>43116</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
+        <v>7.13</v>
+      </c>
+      <c r="C4" s="2">
         <v>5.74</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D4" s="2">
         <v>7.57</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>43115</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
+        <v>6.05</v>
+      </c>
+      <c r="C5" s="2">
         <v>7.93</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="2">
         <v>9.86</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43114</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C6" s="2">
         <v>10.050000000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>9.44</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43113</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="C7" s="2">
         <v>2.97</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>2.96</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>1.19</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43112</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>-2.54</v>
+      </c>
+      <c r="C8" s="2">
         <v>-4.29</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>-4.58</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>-1.76</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>-3.11</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43111</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>-9.01</v>
+      </c>
+      <c r="C9" s="2">
         <v>-8.25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>-8.76</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>-5.31</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
         <v>43110</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>-5.97</v>
+      </c>
+      <c r="C10" s="2">
         <v>-5.99</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>-5.99</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>-1.89</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>4.54</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>-1.19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43109</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-3.68</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-3.28</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-1.65</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="2">
-        <v>-3.22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>43108</v>
       </c>
       <c r="B11" s="2">
         <f>SUM(B2:B10)</f>
+        <v>29.200000000000003</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-3.68</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-3.28</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-1.65</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-3.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>43108</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="2">
+        <f>SUM(C3:C11)</f>
         <v>6.24</v>
       </c>
-      <c r="C11" s="2">
-        <f>SUM(C2:C10)</f>
+      <c r="D12" s="2">
+        <f>SUM(D3:D11)</f>
         <v>8.110000000000003</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>-1.07</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>0.27</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>-4.05</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43107</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="D12" s="2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2">
         <v>6.26</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>5.21</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>3.07</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
         <v>43106</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
         <v>12.27</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>12.63</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>11.89</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43105</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>12.23</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>13.07</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>13.07</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
         <v>43104</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2">
-        <f>SUM(D6:D14)</f>
-        <v>20.27</v>
-      </c>
-      <c r="E15" s="2">
-        <v>11.69</v>
-      </c>
-      <c r="F15" s="2">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>43103</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2">
         <f>SUM(E7:E15)</f>
-        <v>47.05</v>
+        <v>20.27</v>
       </c>
       <c r="F16" s="2">
-        <v>10.27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+        <v>11.69</v>
+      </c>
+      <c r="G16" s="2">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>43103</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="2">
         <f>SUM(F8:F16)</f>
+        <v>47.05</v>
+      </c>
+      <c r="G17" s="2">
+        <v>10.27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="2">
+        <f>SUM(G9:G17)</f>
         <v>38.85</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G9:G17">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="14" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F8:F16">
-    <cfRule type="cellIs" dxfId="47" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="12" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E15">
-    <cfRule type="cellIs" dxfId="45" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D14">
-    <cfRule type="cellIs" dxfId="43" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C15">
-    <cfRule type="cellIs" dxfId="41" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10">
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D16">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D11">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="6" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C11">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2085,546 +2320,623 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="A15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="4" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43122</v>
+        <v>43123</v>
       </c>
       <c r="B2" s="2">
-        <v>-2.93</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-4.07</v>
-      </c>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43121</v>
+        <v>43122</v>
       </c>
       <c r="B3" s="2">
-        <v>-5.67</v>
+        <v>-2.04</v>
       </c>
       <c r="C3" s="2">
-        <v>-6.47</v>
+        <v>-2.93</v>
       </c>
       <c r="D3" s="2">
-        <v>-6.17</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>-4.07</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
+        <v>43121</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-3.79</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-5.67</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-6.47</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-6.17</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>43120</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="2">
+        <v>-5.87</v>
+      </c>
+      <c r="C5" s="2">
         <v>-8.2200000000000006</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D5" s="2">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E5" s="2">
         <v>-8.44</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43119</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="C6" s="2">
         <v>-7.44</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>-9.09</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>-9.1</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43118</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>3.03</v>
+      </c>
+      <c r="C7" s="2">
         <v>-1.7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>-4.87</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>-9.01</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>-7.22</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43117</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>6.38</v>
+      </c>
+      <c r="C8" s="2">
         <v>4.28</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>0.4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>-1.77</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>-4.34</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>-5.25</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="H8" s="2"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43116</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>6.04</v>
+      </c>
+      <c r="C9" s="2">
         <v>7.11</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>5.13</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>3.7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>-0.59</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-2.1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-3.32</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
         <v>-0.98</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J9" s="2">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="9" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+    <row r="10" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43115</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>5.63</v>
+      </c>
+      <c r="C10" s="2">
         <v>7.99</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>8.14</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>7.99</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>2.73</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>1.07</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>0.05</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <v>1.6</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J10" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+    <row r="11" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43114</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>9.08</v>
+      </c>
+      <c r="C11" s="2">
         <v>9.26</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>8.92</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>8.39</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>4.32</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>3.59</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>2.62</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <v>3.37</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J11" s="2">
         <v>4.62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>43113</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="C12" s="2">
         <v>3.06</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>3.02</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>2.16</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>3.63</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>2.06</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <v>2.59</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J12" s="2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43112</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>-2.56</v>
+      </c>
+      <c r="C13" s="2">
         <v>-4</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>-3.95</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>-4.3099999999999996</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>-0.08</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>0.46</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>1.44</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <v>1.58</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J13" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="13" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43111</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
+        <v>-8.75</v>
+      </c>
+      <c r="C14" s="2">
         <v>-8.1300000000000008</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="2">
         <v>-8.5299999999999994</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>-7.86</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>-5.05</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>-3.31</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>2.34</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <v>0.63</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J14" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43110</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>-5.91</v>
+      </c>
+      <c r="C15" s="2">
         <v>-5.58</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>-5.64</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>-4.5</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>-3.68</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>-2.74</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J15" s="2">
         <v>1.63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43109</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-3.51</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-3.11</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-2.31</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-2.34</v>
-      </c>
-      <c r="F15" s="2">
-        <v>-1.72</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-0.82</v>
-      </c>
-      <c r="H15" s="2">
-        <v>-0.25</v>
-      </c>
-      <c r="I15" s="2">
-        <v>-1.66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>43108</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
+        <v>4.18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-3.51</v>
+      </c>
+      <c r="D16" s="2">
+        <v>-3.11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-2.31</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-2.34</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-1.72</v>
+      </c>
+      <c r="H16" s="2">
+        <v>-0.82</v>
+      </c>
+      <c r="I16" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="J16" s="2">
+        <v>-1.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>43108</v>
+      </c>
+      <c r="C17" s="2">
+        <f>SUM(C3:C16)</f>
         <v>-15.48</v>
-      </c>
-      <c r="C16" s="2">
-        <f>SUM(C2:C15)</f>
-        <v>-28.82</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-1.3</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-1.1100000000000001</v>
-      </c>
-      <c r="F16" s="2">
-        <v>-0.92</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-0.84</v>
-      </c>
-      <c r="H16" s="2">
-        <v>-1.61</v>
-      </c>
-      <c r="I16" s="2">
-        <v>-3.16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <v>43107</v>
       </c>
       <c r="D17" s="2">
         <f>SUM(D3:D16)</f>
+        <v>-28.82</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-1.3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-0.92</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-0.84</v>
+      </c>
+      <c r="I17" s="2">
+        <v>-1.61</v>
+      </c>
+      <c r="J17" s="2">
+        <v>-3.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>43107</v>
+      </c>
+      <c r="E18" s="2">
+        <f>SUM(E4:E17)</f>
         <v>-32.53</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F18" s="2">
         <v>6.29</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G18" s="2">
         <v>6.25</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H18" s="2">
         <v>5.26</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I18" s="2">
         <v>3.76</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J18" s="2">
         <v>2.85</v>
       </c>
     </row>
-    <row r="18" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+    <row r="19" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
         <v>43106</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F19" s="2">
         <v>12.56</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G19" s="2">
         <v>12.6</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H19" s="2">
         <v>13.02</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I19" s="2">
         <v>12.61</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J19" s="2">
         <v>12.42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    <row r="20" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
         <v>43105</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F20" s="2">
         <v>12.51</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G20" s="2">
         <v>12.64</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H20" s="2">
         <v>13.24</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I20" s="2">
         <v>13.38</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J20" s="2">
         <v>13.55</v>
       </c>
     </row>
-    <row r="20" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    <row r="21" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
         <v>43104</v>
-      </c>
-      <c r="E20" s="2">
-        <f>SUM(E6:E19)</f>
-        <v>16.470000000000002</v>
-      </c>
-      <c r="F20" s="2">
-        <v>11.71</v>
-      </c>
-      <c r="G20" s="2">
-        <v>11.91</v>
-      </c>
-      <c r="H20" s="2">
-        <v>11.84</v>
-      </c>
-      <c r="I20" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
-        <v>43103</v>
       </c>
       <c r="F21" s="2">
         <f>SUM(F7:F20)</f>
+        <v>16.470000000000002</v>
+      </c>
+      <c r="G21" s="2">
+        <v>11.71</v>
+      </c>
+      <c r="H21" s="2">
+        <v>11.91</v>
+      </c>
+      <c r="I21" s="2">
+        <v>11.84</v>
+      </c>
+      <c r="J21" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>43103</v>
+      </c>
+      <c r="G22" s="2">
+        <f>SUM(G8:G21)</f>
         <v>35.909999999999997</v>
       </c>
-      <c r="G21" s="2">
-        <f>SUM(G7:G20)</f>
-        <v>49.22</v>
-      </c>
-      <c r="H21" s="2">
-        <v>10.97</v>
-      </c>
-      <c r="I21" s="2">
-        <v>10.72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H22" s="2">
         <f>SUM(H8:H21)</f>
+        <v>49.22</v>
+      </c>
+      <c r="I22" s="2">
+        <v>10.97</v>
+      </c>
+      <c r="J22" s="2">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="2">
+        <f>SUM(I9:I22)</f>
         <v>60.58</v>
       </c>
-      <c r="I22" s="2">
-        <f>SUM(I8:I21)</f>
+      <c r="J23" s="2">
+        <f>SUM(J9:J22)</f>
         <v>59.83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:10" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="H8:I21">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="I9:J22">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I22">
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8:H21">
+    <cfRule type="cellIs" dxfId="35" priority="31" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2636,7 +2948,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G20">
+  <conditionalFormatting sqref="G8:G21">
     <cfRule type="cellIs" dxfId="31" priority="27" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2644,7 +2956,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G20">
+  <conditionalFormatting sqref="G8:G21">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2652,7 +2964,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F20">
+  <conditionalFormatting sqref="F11:F20">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2660,7 +2972,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F20">
+  <conditionalFormatting sqref="F11:F20">
     <cfRule type="cellIs" dxfId="25" priority="21" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2668,7 +2980,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E19">
+  <conditionalFormatting sqref="E4:F10">
     <cfRule type="cellIs" dxfId="23" priority="19" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2676,7 +2988,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E19">
+  <conditionalFormatting sqref="E4:F10">
     <cfRule type="cellIs" dxfId="21" priority="17" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2684,7 +2996,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E9">
+  <conditionalFormatting sqref="E11:E17">
     <cfRule type="cellIs" dxfId="19" priority="15" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2692,7 +3004,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:E9">
+  <conditionalFormatting sqref="E11:E17">
     <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2700,7 +3012,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D16">
+  <conditionalFormatting sqref="D3:D16">
     <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2708,7 +3020,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D16">
+  <conditionalFormatting sqref="D3:D16">
     <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2716,7 +3028,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C15">
+  <conditionalFormatting sqref="C3:C16">
     <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2724,7 +3036,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C15">
+  <conditionalFormatting sqref="C3:C16">
     <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>

</xml_diff>

<commit_message>
update GFS on 201801111258
</commit_message>
<xml_diff>
--- a/GFS/GFS.xlsx
+++ b/GFS/GFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GFS-HDD" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>2018-01-02 12z</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>2018-01-10 00z</t>
+  </si>
+  <si>
+    <t>2018-01-11 12z</t>
+  </si>
+  <si>
+    <t>2018-01-11 00z</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,75 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -1160,60 +1234,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="E17:J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43125</v>
+        <v>43126</v>
       </c>
       <c r="B2" s="2">
-        <v>-6.08</v>
+        <v>-3.84</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1223,16 +1300,17 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43124</v>
+        <v>43125</v>
       </c>
       <c r="B3" s="2">
-        <v>-1.9</v>
+        <v>-0.33</v>
       </c>
       <c r="C3" s="2">
-        <v>5.57</v>
+        <v>-6.08</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1241,665 +1319,735 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43123</v>
+        <v>43124</v>
       </c>
       <c r="B4" s="2">
-        <v>-0.34</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="C4" s="2">
-        <v>6.14</v>
+        <v>-1.9</v>
       </c>
       <c r="D4" s="2">
-        <v>3.69</v>
-      </c>
-      <c r="E4" s="2">
-        <v>-0.26</v>
-      </c>
+        <v>5.57</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
+        <v>43123</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-0.34</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.14</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-0.26</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43122</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>-0.64</v>
+      </c>
+      <c r="C6" s="2">
         <v>-3.93</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>2.0299999999999998</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>4.8899999999999997</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F6" s="2">
         <v>4.21</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G6" s="2">
         <v>1.91</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43121</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>-4.88</v>
+      </c>
+      <c r="C7" s="2">
         <v>-8.11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>-6.26</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>-0.56999999999999995</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>2.71</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G7" s="2">
         <v>-0.15</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43120</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>-5.29</v>
+      </c>
+      <c r="C8" s="2">
         <v>-10.65</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>-9.06</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>-4.7300000000000004</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>-0.85</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43119</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>2.34</v>
+      </c>
+      <c r="C9" s="2">
         <v>-8.5500000000000007</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>-5.84</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>-5.59</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>-7.41</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>3.11</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-10.98</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
         <v>-10.28</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43118</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>8.81</v>
+      </c>
+      <c r="C10" s="2">
         <v>-1.61</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>-2.06</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>-8.9499999999999993</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>6.76</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>-10.48</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <v>-6.81</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J10" s="2">
         <v>-9.3699999999999992</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43117</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>9.69</v>
+      </c>
+      <c r="C11" s="2">
         <v>5.99</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>7.69</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>6.01</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>-8.8699999999999992</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>1.81</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>-8.9</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <v>-0.99</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J11" s="2">
         <v>-8.0299999999999994</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K11" s="2">
         <v>-6.55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>43116</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>6.82</v>
+      </c>
+      <c r="C12" s="2">
         <v>6.75</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>7.21</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>7.9</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>4.46</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>-4.1100000000000003</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <v>3.95</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J12" s="2">
         <v>-6.26</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K12" s="2">
         <v>-3.58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43115</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="C13" s="2">
         <v>5.03</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>5.91</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>6.24</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>6.49</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>9.85</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>-1.5</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J13" s="2">
         <v>-2.0099999999999998</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K13" s="2">
         <v>-0.43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43114</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
+        <v>6.47</v>
+      </c>
+      <c r="C14" s="2">
         <v>6.5</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D14" s="2">
         <v>7.16</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>6.74</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>9.66</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>9.44</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>-1.01</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <v>2.29</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J14" s="2">
         <v>-0.09</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K14" s="2">
         <v>1.26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43113</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>4.21</v>
+      </c>
+      <c r="C15" s="2">
         <v>2.48</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>2.66</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>4.0599999999999996</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>2.95</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>-0.66</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J15" s="2">
         <v>-1.43</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K15" s="2">
         <v>5.64</v>
       </c>
     </row>
-    <row r="15" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43112</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="2">
+        <v>-3.55</v>
+      </c>
+      <c r="C16" s="2">
         <v>-4.12</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D16" s="2">
         <v>-4.38</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E16" s="2">
         <v>-3.93</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F16" s="2">
         <v>-3.42</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G16" s="2">
         <v>-3.84</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H16" s="2">
         <v>2.38</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I16" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J16" s="2">
         <v>-3.52</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K16" s="2">
         <v>4.54</v>
       </c>
     </row>
-    <row r="16" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+    <row r="17" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
         <v>43111</v>
-      </c>
-      <c r="B16" s="2">
-        <v>-9.23</v>
-      </c>
-      <c r="C16" s="2">
-        <v>-8.7799999999999994</v>
-      </c>
-      <c r="D16" s="2">
-        <v>-8.61</v>
-      </c>
-      <c r="E16" s="2">
-        <v>-8.68</v>
-      </c>
-      <c r="F16" s="2">
-        <v>-8.33</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-4.13</v>
-      </c>
-      <c r="H16" s="2">
-        <v>-4.57</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="J16" s="2">
-        <v>-1.06</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <v>43110</v>
       </c>
       <c r="B17" s="7">
         <f>SUM(B2:B16)</f>
-        <v>-27.77</v>
+        <v>31.37</v>
       </c>
       <c r="C17" s="2">
-        <v>-6.68</v>
+        <v>-9.23</v>
       </c>
       <c r="D17" s="2">
-        <v>-6.92</v>
+        <v>-8.7799999999999994</v>
       </c>
       <c r="E17" s="2">
-        <v>-7.18</v>
+        <v>-8.61</v>
       </c>
       <c r="F17" s="2">
-        <v>-6.81</v>
+        <v>-8.68</v>
       </c>
       <c r="G17" s="2">
-        <v>-3.96</v>
+        <v>-8.33</v>
       </c>
       <c r="H17" s="2">
-        <v>-2.85</v>
+        <v>-4.13</v>
       </c>
       <c r="I17" s="2">
-        <v>2.44</v>
+        <v>-4.57</v>
       </c>
       <c r="J17" s="2">
-        <v>3.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.31</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-1.06</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>43109</v>
-      </c>
-      <c r="B18" s="8"/>
+        <v>43110</v>
+      </c>
       <c r="C18" s="7">
         <f>SUM(C3:C17)</f>
-        <v>4.1200000000000028</v>
+        <v>-27.77</v>
       </c>
       <c r="D18" s="2">
-        <v>-4.1500000000000004</v>
+        <v>-6.68</v>
       </c>
       <c r="E18" s="2">
-        <v>-3.79</v>
+        <v>-6.92</v>
       </c>
       <c r="F18" s="2">
-        <v>-3.69</v>
+        <v>-7.18</v>
       </c>
       <c r="G18" s="2">
-        <v>-2.52</v>
+        <v>-6.81</v>
       </c>
       <c r="H18" s="2">
-        <v>-2.36</v>
+        <v>-3.96</v>
       </c>
       <c r="I18" s="2">
-        <v>-3.49</v>
+        <v>-2.85</v>
       </c>
       <c r="J18" s="2">
-        <v>-3.86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2.44</v>
+      </c>
+      <c r="K18" s="2">
+        <v>3.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>43108</v>
-      </c>
-      <c r="B19" s="8"/>
+        <v>43109</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="D19" s="7">
         <f>SUM(D4:D18)</f>
-        <v>1.1999999999999993</v>
-      </c>
-      <c r="E19" s="7">
-        <f>SUM(E4:E18)</f>
-        <v>-28.169999999999991</v>
+        <v>4.1200000000000028</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-4.1500000000000004</v>
       </c>
       <c r="F19" s="2">
-        <v>-1.91</v>
+        <v>-3.79</v>
       </c>
       <c r="G19" s="2">
-        <v>-3.15</v>
+        <v>-3.69</v>
       </c>
       <c r="H19" s="2">
-        <v>-3.31</v>
+        <v>-2.52</v>
       </c>
       <c r="I19" s="2">
-        <v>-2.99</v>
+        <v>-2.36</v>
       </c>
       <c r="J19" s="2">
-        <v>-5.51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-3.49</v>
+      </c>
+      <c r="K19" s="2">
+        <v>-3.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>43107</v>
-      </c>
-      <c r="B20" s="8"/>
+        <v>43108</v>
+      </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
+      <c r="E20" s="7">
+        <f>SUM(E5:E19)</f>
+        <v>1.1999999999999993</v>
+      </c>
       <c r="F20" s="7">
         <f>SUM(F5:F19)</f>
-        <v>14.710000000000004</v>
+        <v>-28.169999999999991</v>
       </c>
       <c r="G20" s="2">
-        <v>2.94</v>
+        <v>-1.91</v>
       </c>
       <c r="H20" s="2">
-        <v>3.32</v>
+        <v>-3.15</v>
       </c>
       <c r="I20" s="2">
-        <v>3.79</v>
+        <v>-3.31</v>
       </c>
       <c r="J20" s="2">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-2.99</v>
+      </c>
+      <c r="K20" s="2">
+        <v>-5.51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>43106</v>
-      </c>
-      <c r="B21" s="8"/>
+        <v>43107</v>
+      </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="G21" s="2">
-        <v>9.02</v>
+      <c r="E21" s="8"/>
+      <c r="G21" s="7">
+        <f>SUM(G6:G20)</f>
+        <v>14.710000000000004</v>
       </c>
       <c r="H21" s="2">
-        <v>9.2799999999999994</v>
+        <v>2.94</v>
       </c>
       <c r="I21" s="2">
-        <v>9.9600000000000009</v>
+        <v>3.32</v>
       </c>
       <c r="J21" s="2">
-        <v>9.36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3.79</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
-        <v>43105</v>
-      </c>
-      <c r="B22" s="8"/>
+        <v>43106</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="G22" s="2">
-        <v>9.92</v>
-      </c>
+      <c r="E22" s="8"/>
       <c r="H22" s="2">
-        <v>10.26</v>
+        <v>9.02</v>
       </c>
       <c r="I22" s="2">
-        <v>10.46</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="J22" s="2">
-        <v>10.94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="K22" s="2">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
-        <v>43104</v>
-      </c>
-      <c r="B23" s="8"/>
+        <v>43105</v>
+      </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="G23" s="7">
-        <f>SUM(G8:G22)</f>
-        <v>-27.14</v>
-      </c>
-      <c r="H23" s="7">
-        <f>SUM(H8:H22)</f>
-        <v>2.7300000000000004</v>
+      <c r="E23" s="8"/>
+      <c r="H23" s="2">
+        <v>9.92</v>
       </c>
       <c r="I23" s="2">
-        <v>10.199999999999999</v>
+        <v>10.26</v>
       </c>
       <c r="J23" s="2">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>10.46</v>
+      </c>
+      <c r="K23" s="2">
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
-        <v>43103</v>
-      </c>
-      <c r="B24" s="8"/>
+        <v>43104</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="I24" s="2">
+      <c r="E24" s="8"/>
+      <c r="H24" s="7">
+        <f>SUM(H9:H23)</f>
+        <v>-27.14</v>
+      </c>
+      <c r="I24" s="7">
         <f>SUM(I9:I23)</f>
-        <v>-2.9999999999997584E-2</v>
+        <v>2.7300000000000004</v>
       </c>
       <c r="J24" s="2">
-        <v>9.6300000000000008</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K24" s="2">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4">
+        <v>43103</v>
+      </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="I25" s="7"/>
+      <c r="E25" s="8"/>
       <c r="J25" s="2">
         <f>SUM(J10:J24)</f>
+        <v>-2.9999999999997584E-2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>9.6300000000000008</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="2">
+        <f>SUM(K11:K25)</f>
         <v>35.020000000000003</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K11:K25">
+    <cfRule type="cellIs" dxfId="83" priority="23" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="24" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J10:J24">
-    <cfRule type="cellIs" dxfId="75" priority="21" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="22" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="81" priority="21" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="22" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I23">
-    <cfRule type="cellIs" dxfId="73" priority="19" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="20" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H22">
-    <cfRule type="cellIs" dxfId="71" priority="17" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="18" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G22">
-    <cfRule type="cellIs" dxfId="69" priority="15" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="16" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F19 F21:F22">
-    <cfRule type="cellIs" dxfId="67" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="14" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4:H18 E21:H22 F19:H19 E20 G20:H20 E24:H1048576 E23:F23">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E24">
-    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E24">
-    <cfRule type="cellIs" dxfId="61" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="79" priority="19" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="20" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:H23">
+    <cfRule type="cellIs" dxfId="77" priority="17" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="18" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:G20 G22:G23">
+    <cfRule type="cellIs" dxfId="75" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:I19 F22:I23 G20:I20 F21 H21:I21 F25:I1048576 F24:G24">
+    <cfRule type="cellIs" dxfId="73" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="14" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F25">
+    <cfRule type="cellIs" dxfId="71" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F25">
+    <cfRule type="cellIs" dxfId="69" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E19">
+    <cfRule type="cellIs" dxfId="67" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="8" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D18">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B16">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1910,406 +2058,468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
+        <v>43119</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.86</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>43118</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
+        <v>7.07</v>
+      </c>
+      <c r="C3" s="2">
         <v>7.46</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>43117</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10.86</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.76</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.89</v>
-      </c>
+      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43116</v>
+        <v>43117</v>
       </c>
       <c r="B4" s="2">
-        <v>7.13</v>
+        <v>10.08</v>
       </c>
       <c r="C4" s="2">
-        <v>5.74</v>
+        <v>10.86</v>
       </c>
       <c r="D4" s="2">
-        <v>7.57</v>
-      </c>
-      <c r="E4" s="9"/>
+        <v>1.76</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.89</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>43115</v>
+        <v>43116</v>
       </c>
       <c r="B5" s="2">
-        <v>6.05</v>
+        <v>8.44</v>
       </c>
       <c r="C5" s="2">
-        <v>7.93</v>
+        <v>7.13</v>
       </c>
       <c r="D5" s="2">
-        <v>9.86</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>5.74</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7.57</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>43114</v>
+        <v>43115</v>
       </c>
       <c r="B6" s="2">
-        <v>9.1999999999999993</v>
+        <v>6.11</v>
       </c>
       <c r="C6" s="2">
-        <v>10.050000000000001</v>
+        <v>6.05</v>
       </c>
       <c r="D6" s="2">
-        <v>9.44</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>7.93</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.86</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>43113</v>
+        <v>43114</v>
       </c>
       <c r="B7" s="2">
-        <v>6.02</v>
+        <v>9.24</v>
       </c>
       <c r="C7" s="2">
-        <v>2.97</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D7" s="2">
-        <v>2.96</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E7" s="2">
-        <v>1.19</v>
+        <v>9.44</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
+        <v>43113</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6.02</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.97</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.96</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43112</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>-2.56</v>
+      </c>
+      <c r="C9" s="2">
         <v>-2.54</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>-4.29</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>-4.58</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>-1.76</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-3.11</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43111</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>-9.0299999999999994</v>
+      </c>
+      <c r="C10" s="2">
         <v>-9.01</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>-8.25</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>-8.76</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>-5.31</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>-2.5099999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
         <v>43110</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-5.97</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-5.99</v>
-      </c>
-      <c r="D10" s="2">
-        <v>-5.99</v>
-      </c>
-      <c r="E10" s="2">
-        <v>-1.89</v>
-      </c>
-      <c r="F10" s="2">
-        <v>4.54</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-1.19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>43109</v>
       </c>
       <c r="B11" s="2">
         <f>SUM(B2:B10)</f>
-        <v>29.200000000000003</v>
+        <v>38.459999999999994</v>
       </c>
       <c r="C11" s="2">
-        <v>-3.68</v>
+        <v>-5.97</v>
       </c>
       <c r="D11" s="2">
-        <v>-3.28</v>
+        <v>-5.99</v>
       </c>
       <c r="E11" s="2">
-        <v>-1.65</v>
+        <v>-5.99</v>
       </c>
       <c r="F11" s="2">
-        <v>0.2</v>
+        <v>-1.89</v>
       </c>
       <c r="G11" s="2">
-        <v>-3.22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
-        <v>43108</v>
-      </c>
-      <c r="B12" s="10"/>
+        <v>4.54</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-1.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>43109</v>
+      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="2">
         <f>SUM(C3:C11)</f>
+        <v>29.200000000000003</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-3.68</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-3.28</v>
+      </c>
+      <c r="F12" s="2">
+        <v>-1.65</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-3.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>43108</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="2">
+        <f>SUM(D4:D12)</f>
         <v>6.24</v>
       </c>
-      <c r="D12" s="2">
-        <f>SUM(D3:D11)</f>
+      <c r="E13" s="2">
+        <f>SUM(E4:E12)</f>
         <v>8.110000000000003</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>-1.07</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>0.27</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>-4.05</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43107</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="2">
         <v>6.26</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>5.21</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>3.07</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
         <v>43106</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
         <v>12.27</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>12.63</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>11.89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43105</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
         <v>12.23</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G16" s="2">
         <v>13.07</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H16" s="2">
         <v>13.07</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
         <v>43104</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <f>SUM(E7:E15)</f>
-        <v>20.27</v>
-      </c>
-      <c r="F16" s="2">
-        <v>11.69</v>
-      </c>
-      <c r="G16" s="2">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <v>43103</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2">
         <f>SUM(F8:F16)</f>
-        <v>47.05</v>
+        <v>20.27</v>
       </c>
       <c r="G17" s="2">
-        <v>10.27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+        <v>11.69</v>
+      </c>
+      <c r="H17" s="2">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>43103</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="2">
         <f>SUM(G9:G17)</f>
+        <v>47.05</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="2">
+        <f>SUM(H10:H18)</f>
         <v>38.85</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H10:H18">
+    <cfRule type="cellIs" dxfId="59" priority="15" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="16" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G9:G17">
-    <cfRule type="cellIs" dxfId="53" priority="13" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="13" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="14" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F16">
-    <cfRule type="cellIs" dxfId="51" priority="11" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="12" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E15">
-    <cfRule type="cellIs" dxfId="49" priority="9" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="10" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D16">
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="8" operator="greaterThanOrEqual">
-      <formula>2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D11">
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="11" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="12" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E17">
+    <cfRule type="cellIs" dxfId="53" priority="9" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="10" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E12">
+    <cfRule type="cellIs" dxfId="51" priority="7" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="8" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D12">
+    <cfRule type="cellIs" dxfId="49" priority="5" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="6" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="4" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B10">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2320,59 +2530,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="A15:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="4" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="5" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43123</v>
+        <v>43124</v>
       </c>
       <c r="B2" s="2">
-        <v>-2.2000000000000002</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2380,547 +2593,622 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>43122</v>
+        <v>43123</v>
       </c>
       <c r="B3" s="2">
-        <v>-2.04</v>
+        <v>-2.85</v>
       </c>
       <c r="C3" s="2">
-        <v>-2.93</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-4.07</v>
-      </c>
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>43121</v>
+        <v>43122</v>
       </c>
       <c r="B4" s="2">
-        <v>-3.79</v>
+        <v>-2.2400000000000002</v>
       </c>
       <c r="C4" s="2">
-        <v>-5.67</v>
+        <v>-2.04</v>
       </c>
       <c r="D4" s="2">
-        <v>-6.47</v>
+        <v>-2.93</v>
       </c>
       <c r="E4" s="2">
-        <v>-6.17</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>-4.07</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
+        <v>43121</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-4.5199999999999996</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-3.79</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-5.67</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-6.47</v>
+      </c>
+      <c r="F5" s="2">
+        <v>-6.17</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>43120</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
+        <v>-4.09</v>
+      </c>
+      <c r="C6" s="2">
         <v>-5.87</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D6" s="2">
         <v>-8.2200000000000006</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E6" s="2">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F6" s="2">
         <v>-8.44</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>43119</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="C7" s="2">
         <v>-1.1599999999999999</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D7" s="2">
         <v>-7.44</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E7" s="2">
         <v>-9.09</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F7" s="2">
         <v>-9.1</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>43118</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
+        <v>7.21</v>
+      </c>
+      <c r="C8" s="2">
         <v>3.03</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D8" s="2">
         <v>-1.7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E8" s="2">
         <v>-4.87</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F8" s="2">
         <v>-9.01</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G8" s="2">
         <v>-7.22</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>43117</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
+        <v>10.73</v>
+      </c>
+      <c r="C9" s="2">
         <v>6.38</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D9" s="2">
         <v>4.28</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E9" s="2">
         <v>0.4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F9" s="2">
         <v>-1.77</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G9" s="2">
         <v>-4.34</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H9" s="2">
         <v>-5.25</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
+      <c r="I9" s="2"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>43116</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
+        <v>8.81</v>
+      </c>
+      <c r="C10" s="2">
         <v>6.04</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D10" s="2">
         <v>7.11</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E10" s="2">
         <v>5.13</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F10" s="2">
         <v>3.7</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G10" s="2">
         <v>-0.59</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H10" s="2">
         <v>-2.1</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <v>-3.32</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J10" s="2">
         <v>-0.98</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K10" s="2">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="10" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+    <row r="11" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>43115</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="C11" s="2">
         <v>5.63</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D11" s="2">
         <v>7.99</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E11" s="2">
         <v>8.14</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F11" s="2">
         <v>7.99</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G11" s="2">
         <v>2.73</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H11" s="2">
         <v>1.07</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <v>0.05</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J11" s="2">
         <v>1.6</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K11" s="2">
         <v>2.48</v>
       </c>
     </row>
-    <row r="11" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>43114</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C12" s="2">
         <v>9.08</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D12" s="2">
         <v>9.26</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>8.92</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F12" s="2">
         <v>8.39</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>4.32</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>3.59</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <v>2.62</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J12" s="2">
         <v>3.37</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K12" s="2">
         <v>4.62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+    <row r="13" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
         <v>43113</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B13" s="2">
+        <v>6.31</v>
+      </c>
+      <c r="C13" s="2">
         <v>6.3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D13" s="2">
         <v>3.06</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E13" s="2">
         <v>3.02</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F13" s="2">
         <v>2.16</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G13" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H13" s="2">
         <v>3.63</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <v>2.06</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J13" s="2">
         <v>2.59</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K13" s="2">
         <v>3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+    <row r="14" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
         <v>43112</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B14" s="2">
         <v>-2.56</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="2">
+        <v>-2.56</v>
+      </c>
+      <c r="D14" s="2">
         <v>-4</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E14" s="2">
         <v>-3.95</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F14" s="2">
         <v>-4.3099999999999996</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G14" s="2">
         <v>-0.08</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H14" s="2">
         <v>0.46</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <v>1.44</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J14" s="2">
         <v>1.58</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K14" s="2">
         <v>0.86</v>
       </c>
     </row>
-    <row r="14" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+    <row r="15" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
         <v>43111</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B15" s="2">
+        <v>-8.9700000000000006</v>
+      </c>
+      <c r="C15" s="2">
         <v>-8.75</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D15" s="2">
         <v>-8.1300000000000008</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E15" s="2">
         <v>-8.5299999999999994</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F15" s="2">
         <v>-7.86</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G15" s="2">
         <v>-5.05</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H15" s="2">
         <v>-3.31</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <v>2.34</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J15" s="2">
         <v>0.63</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K15" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+    <row r="16" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
         <v>43110</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-5.91</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-5.58</v>
-      </c>
-      <c r="D15" s="2">
-        <v>-5.64</v>
-      </c>
-      <c r="E15" s="2">
-        <v>-4.5</v>
-      </c>
-      <c r="F15" s="2">
-        <v>-3.68</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-2.74</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>43109</v>
       </c>
       <c r="B16" s="2">
         <f>SUM(B2:B15)</f>
-        <v>4.18</v>
+        <v>20.550000000000004</v>
       </c>
       <c r="C16" s="2">
-        <v>-3.51</v>
+        <v>-5.91</v>
       </c>
       <c r="D16" s="2">
-        <v>-3.11</v>
+        <v>-5.58</v>
       </c>
       <c r="E16" s="2">
-        <v>-2.31</v>
+        <v>-5.64</v>
       </c>
       <c r="F16" s="2">
-        <v>-2.34</v>
+        <v>-4.5</v>
       </c>
       <c r="G16" s="2">
-        <v>-1.72</v>
+        <v>-3.68</v>
       </c>
       <c r="H16" s="2">
-        <v>-0.82</v>
+        <v>-2.74</v>
       </c>
       <c r="I16" s="2">
-        <v>-0.25</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J16" s="2">
-        <v>-1.66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
-        <v>43108</v>
+        <v>43109</v>
       </c>
       <c r="C17" s="2">
         <f>SUM(C3:C16)</f>
+        <v>4.18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-3.51</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-3.11</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-2.31</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-2.34</v>
+      </c>
+      <c r="H17" s="2">
+        <v>-1.72</v>
+      </c>
+      <c r="I17" s="2">
+        <v>-0.82</v>
+      </c>
+      <c r="J17" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-1.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>43108</v>
+      </c>
+      <c r="D18" s="2">
+        <f>SUM(D4:D17)</f>
         <v>-15.48</v>
-      </c>
-      <c r="D17" s="2">
-        <f>SUM(D3:D16)</f>
-        <v>-28.82</v>
-      </c>
-      <c r="E17" s="2">
-        <v>-1.3</v>
-      </c>
-      <c r="F17" s="2">
-        <v>-1.1100000000000001</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-0.92</v>
-      </c>
-      <c r="H17" s="2">
-        <v>-0.84</v>
-      </c>
-      <c r="I17" s="2">
-        <v>-1.61</v>
-      </c>
-      <c r="J17" s="2">
-        <v>-3.16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>43107</v>
       </c>
       <c r="E18" s="2">
         <f>SUM(E4:E17)</f>
+        <v>-28.82</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-1.3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>-0.92</v>
+      </c>
+      <c r="I18" s="2">
+        <v>-0.84</v>
+      </c>
+      <c r="J18" s="2">
+        <v>-1.61</v>
+      </c>
+      <c r="K18" s="2">
+        <v>-3.16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>43107</v>
+      </c>
+      <c r="F19" s="2">
+        <f>SUM(F5:F18)</f>
         <v>-32.53</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G19" s="2">
         <v>6.29</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H19" s="2">
         <v>6.25</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I19" s="2">
         <v>5.26</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J19" s="2">
         <v>3.76</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K19" s="2">
         <v>2.85</v>
       </c>
     </row>
-    <row r="19" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+    <row r="20" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
         <v>43106</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G20" s="2">
         <v>12.56</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H20" s="2">
         <v>12.6</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I20" s="2">
         <v>13.02</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J20" s="2">
         <v>12.61</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K20" s="2">
         <v>12.42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+    <row r="21" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
         <v>43105</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G21" s="2">
         <v>12.51</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H21" s="2">
         <v>12.64</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I21" s="2">
         <v>13.24</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J21" s="2">
         <v>13.38</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K21" s="2">
         <v>13.55</v>
       </c>
     </row>
-    <row r="21" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+    <row r="22" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
         <v>43104</v>
-      </c>
-      <c r="F21" s="2">
-        <f>SUM(F7:F20)</f>
-        <v>16.470000000000002</v>
-      </c>
-      <c r="G21" s="2">
-        <v>11.71</v>
-      </c>
-      <c r="H21" s="2">
-        <v>11.91</v>
-      </c>
-      <c r="I21" s="2">
-        <v>11.84</v>
-      </c>
-      <c r="J21" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
-        <v>43103</v>
       </c>
       <c r="G22" s="2">
         <f>SUM(G8:G21)</f>
+        <v>16.470000000000002</v>
+      </c>
+      <c r="H22" s="2">
+        <v>11.71</v>
+      </c>
+      <c r="I22" s="2">
+        <v>11.91</v>
+      </c>
+      <c r="J22" s="2">
+        <v>11.84</v>
+      </c>
+      <c r="K22" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>43103</v>
+      </c>
+      <c r="H23" s="2">
+        <f>SUM(H9:H22)</f>
         <v>35.909999999999997</v>
       </c>
-      <c r="H22" s="2">
-        <f>SUM(H8:H21)</f>
-        <v>49.22</v>
-      </c>
-      <c r="I22" s="2">
-        <v>10.97</v>
-      </c>
-      <c r="J22" s="2">
-        <v>10.72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I23" s="2">
         <f>SUM(I9:I22)</f>
+        <v>49.22</v>
+      </c>
+      <c r="J23" s="2">
+        <v>10.97</v>
+      </c>
+      <c r="K23" s="2">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="2">
+        <f>SUM(J10:J23)</f>
         <v>60.58</v>
       </c>
-      <c r="J23" s="2">
-        <f>SUM(J9:J22)</f>
+      <c r="K24" s="2">
+        <f>SUM(K10:K23)</f>
         <v>59.83</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="I9:J22">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="lessThanOrEqual">
-      <formula>-2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="J10:K23">
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J23">
+    <cfRule type="cellIs" dxfId="41" priority="37" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="greaterThanOrEqual">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:I22">
+    <cfRule type="cellIs" dxfId="39" priority="35" operator="lessThanOrEqual">
+      <formula>-2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="36" operator="greaterThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2932,7 +3220,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H21">
+  <conditionalFormatting sqref="H9:H22">
     <cfRule type="cellIs" dxfId="35" priority="31" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2940,7 +3228,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H21">
+  <conditionalFormatting sqref="H9:H22">
     <cfRule type="cellIs" dxfId="33" priority="29" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2948,7 +3236,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G21">
+  <conditionalFormatting sqref="G12:G21">
     <cfRule type="cellIs" dxfId="31" priority="27" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2956,7 +3244,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G21">
+  <conditionalFormatting sqref="G12:G21">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2964,7 +3252,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F20">
+  <conditionalFormatting sqref="F5:G11">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2972,7 +3260,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F20">
+  <conditionalFormatting sqref="F5:G11">
     <cfRule type="cellIs" dxfId="25" priority="21" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2980,7 +3268,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:F10">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" dxfId="23" priority="19" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2988,7 +3276,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:F10">
+  <conditionalFormatting sqref="F12:F18">
     <cfRule type="cellIs" dxfId="21" priority="17" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -2996,7 +3284,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E17">
+  <conditionalFormatting sqref="E4:E17">
     <cfRule type="cellIs" dxfId="19" priority="15" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -3004,7 +3292,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E17">
+  <conditionalFormatting sqref="E4:E17">
     <cfRule type="cellIs" dxfId="17" priority="13" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -3012,7 +3300,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
+  <conditionalFormatting sqref="D4:D17">
     <cfRule type="cellIs" dxfId="15" priority="11" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>
@@ -3020,7 +3308,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
+  <conditionalFormatting sqref="D4:D17">
     <cfRule type="cellIs" dxfId="13" priority="9" operator="lessThanOrEqual">
       <formula>-2</formula>
     </cfRule>

</xml_diff>